<commit_message>
Pooh Points: final 20260128 -> PD8
</commit_message>
<xml_diff>
--- a/docs/Today_PoohPoints_SEC_ByOwner_2026-01-28.xlsx
+++ b/docs/Today_PoohPoints_SEC_ByOwner_2026-01-28.xlsx
@@ -3121,7 +3121,7 @@
         </is>
       </c>
       <c r="H44" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I44" t="n">
         <v>21</v>
@@ -3130,7 +3130,7 @@
         <v>3</v>
       </c>
       <c r="K44" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L44" t="n">
         <v>0</v>
@@ -9249,7 +9249,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C8" t="n">
         <v>4</v>

</xml_diff>